<commit_message>
Implemented get values from file(excel)
</commit_message>
<xml_diff>
--- a/Database/TestValues.xlsx
+++ b/Database/TestValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utnfrd-my.sharepoint.com/personal/nmamani_frd_utn_edu_ar/Documents/TREND/DemoSylVac/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87929EB2-CB57-4069-974B-092F5317D426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{87929EB2-CB57-4069-974B-092F5317D426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D02635-C778-4050-B8D2-0445BAE09C0C}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{14502665-497A-47B5-A77D-1D9987157A3C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14502665-497A-47B5-A77D-1D9987157A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -454,7 +454,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,282 +478,282 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" cm="1">
         <f t="array" aca="1" ref="A2:B21" ca="1">_xlfn.RANDARRAY(20,2,0,10)</f>
-        <v>0.82767543209173233</v>
+        <v>8.0451341427028318</v>
       </c>
       <c r="B2" s="1">
         <f ca="1"/>
-        <v>1.794639106988873</v>
+        <v>3.237976392252536</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">_xlfn.CONCAT("INSERT INTO Punto (xCoord,yCoord) VALUES ('",ROUND(A2,2),"', '",ROUND(B2,2),"')")</f>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0.83', '1.79')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8,05', '3,24')</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f ca="1"/>
-        <v>8.3594216586828516</v>
+        <v>5.909745680719233</v>
       </c>
       <c r="B3" s="1">
         <f ca="1"/>
-        <v>3.1908949231332855</v>
+        <v>0.53067396041513604</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D20" ca="1" si="0">_xlfn.CONCAT("INSERT INTO Punto (xCoord,yCoord) VALUES ('",ROUND(A3,2),"', '",ROUND(B3,2),"')")</f>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8.36', '3.19')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,91', '0,53')</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f ca="1"/>
-        <v>6.551732575181509</v>
+        <v>7.5620877690761201</v>
       </c>
       <c r="B4" s="1">
         <f ca="1"/>
-        <v>8.9713206754236996</v>
+        <v>4.1310165308749855</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('6.55', '8.97')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,56', '4,13')</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f ca="1"/>
-        <v>3.3863086283496813</v>
+        <v>1.1617913311784474</v>
       </c>
       <c r="B5" s="1">
         <f ca="1"/>
-        <v>7.5732643650972413</v>
+        <v>1.1880147208838956</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3.39', '7.57')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,16', '1,19')</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f ca="1"/>
-        <v>2.2650517523665261</v>
+        <v>9.6202470963632472</v>
       </c>
       <c r="B6" s="1">
         <f ca="1"/>
-        <v>5.5840252375629653</v>
+        <v>5.0116732727571183</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2.27', '5.58')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('9,62', '5,01')</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f ca="1"/>
-        <v>5.5212267394698724</v>
+        <v>8.6832662871155932</v>
       </c>
       <c r="B7" s="1">
         <f ca="1"/>
-        <v>8.1164531517091998</v>
+        <v>0.31433286480186595</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5.52', '8.12')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8,68', '0,31')</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f ca="1"/>
-        <v>3.9071178343676376</v>
+        <v>5.8404636084957193</v>
       </c>
       <c r="B8" s="1">
         <f ca="1"/>
-        <v>2.9088622303308966</v>
+        <v>0.31317850856775564</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3.91', '2.91')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,84', '0,31')</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f ca="1"/>
-        <v>8.4125247129872882</v>
+        <v>4.4588806134588417</v>
       </c>
       <c r="B9" s="1">
         <f ca="1"/>
-        <v>9.73223357682458</v>
+        <v>9.8825428281564829</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8.41', '9.73')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('4,46', '9,88')</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f ca="1"/>
-        <v>2.5142679912794446</v>
+        <v>1.1537924204977958</v>
       </c>
       <c r="B10" s="1">
         <f ca="1"/>
-        <v>9.0639206116524882</v>
+        <v>7.1514396976385406</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2.51', '9.06')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,15', '7,15')</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f ca="1"/>
-        <v>8.5116432124084209</v>
+        <v>2.4792493337756962</v>
       </c>
       <c r="B11" s="1">
         <f ca="1"/>
-        <v>3.6019105305296879</v>
+        <v>5.1721965017034428</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8.51', '3.6')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2,48', '5,17')</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f ca="1"/>
-        <v>8.7159974142050647</v>
+        <v>1.3785517613308418</v>
       </c>
       <c r="B12" s="1">
         <f ca="1"/>
-        <v>8.4467985818756652</v>
+        <v>4.3615340791068853</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8.72', '8.45')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,38', '4,36')</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f ca="1"/>
-        <v>3.6094161369897364</v>
+        <v>5.4975956841310385</v>
       </c>
       <c r="B13" s="1">
         <f ca="1"/>
-        <v>8.4633705118027951</v>
+        <v>2.3492105855771666</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3.61', '8.46')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,5', '2,35')</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f ca="1"/>
-        <v>0.1329030143964065</v>
+        <v>7.2196062460593406</v>
       </c>
       <c r="B14" s="1">
         <f ca="1"/>
-        <v>0.25641561349188358</v>
+        <v>2.2830419597811193</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0.13', '0.26')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,22', '2,28')</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f ca="1"/>
-        <v>4.3382988815419541</v>
+        <v>0.83257738895471967</v>
       </c>
       <c r="B15" s="1">
         <f ca="1"/>
-        <v>6.9887261835440331</v>
+        <v>0.68417476986563663</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('4.34', '6.99')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,83', '0,68')</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f ca="1"/>
-        <v>8.2867973023472459</v>
+        <v>0.40974657207961407</v>
       </c>
       <c r="B16" s="1">
         <f ca="1"/>
-        <v>1.8243381673012884</v>
+        <v>5.8050724421605722</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8.29', '1.82')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,41', '5,81')</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f ca="1"/>
-        <v>3.9132675865256346</v>
+        <v>1.1443823984450283</v>
       </c>
       <c r="B17" s="1">
         <f ca="1"/>
-        <v>7.6484391267430123</v>
+        <v>2.8006551805361877</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3.91', '7.65')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,14', '2,8')</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f ca="1"/>
-        <v>7.8695404318626032</v>
+        <v>5.8815826736123551</v>
       </c>
       <c r="B18" s="1">
         <f ca="1"/>
-        <v>7.2281838507990308</v>
+        <v>6.7608514001746371</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7.87', '7.23')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,88', '6,76')</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f ca="1"/>
-        <v>6.7760923546661189E-2</v>
+        <v>5.5798722328422183</v>
       </c>
       <c r="B19" s="1">
         <f ca="1"/>
-        <v>9.5821880517846765</v>
+        <v>0.58338364690580136</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0.07', '9.58')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,58', '0,58')</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f ca="1"/>
-        <v>4.6619226795328945</v>
+        <v>6.9060563008237708</v>
       </c>
       <c r="B20" s="1">
         <f ca="1"/>
-        <v>1.8448287007560324</v>
+        <v>1.8253006400313758</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('4.66', '1.84')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('6,91', '1,83')</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f ca="1"/>
-        <v>2.8061494818305359</v>
+        <v>1.4072535534143213</v>
       </c>
       <c r="B21" s="1">
         <f ca="1"/>
-        <v>1.1133866304845466</v>
+        <v>2.2513880605009096</v>
       </c>
       <c r="D21" t="str">
         <f ca="1">_xlfn.CONCAT("INSERT INTO Punto (xCoord,yCoord) VALUES ('",ROUND(A21,2),"', '",ROUND(B21,2),"')")</f>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2.81', '1.11')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,41', '2,25')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new excel file and chart draw from values
</commit_message>
<xml_diff>
--- a/Database/TestValues.xlsx
+++ b/Database/TestValues.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{87929EB2-CB57-4069-974B-092F5317D426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15D02635-C778-4050-B8D2-0445BAE09C0C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14502665-497A-47B5-A77D-1D9987157A3C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{14502665-497A-47B5-A77D-1D9987157A3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -478,282 +478,282 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" cm="1">
         <f t="array" aca="1" ref="A2:B21" ca="1">_xlfn.RANDARRAY(20,2,0,10)</f>
-        <v>8.0451341427028318</v>
+        <v>7.3653252901019624</v>
       </c>
       <c r="B2" s="1">
         <f ca="1"/>
-        <v>3.237976392252536</v>
+        <v>1.8818670881323758</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">_xlfn.CONCAT("INSERT INTO Punto (xCoord,yCoord) VALUES ('",ROUND(A2,2),"', '",ROUND(B2,2),"')")</f>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8,05', '3,24')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,37', '1,88')</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f ca="1"/>
-        <v>5.909745680719233</v>
+        <v>5.0241565429558293</v>
       </c>
       <c r="B3" s="1">
         <f ca="1"/>
-        <v>0.53067396041513604</v>
+        <v>3.4864991536855481</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D20" ca="1" si="0">_xlfn.CONCAT("INSERT INTO Punto (xCoord,yCoord) VALUES ('",ROUND(A3,2),"', '",ROUND(B3,2),"')")</f>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,91', '0,53')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,02', '3,49')</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f ca="1"/>
-        <v>7.5620877690761201</v>
+        <v>2.6273421710034697</v>
       </c>
       <c r="B4" s="1">
         <f ca="1"/>
-        <v>4.1310165308749855</v>
+        <v>9.8984087718393514</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,56', '4,13')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2,63', '9,9')</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f ca="1"/>
-        <v>1.1617913311784474</v>
+        <v>3.6283110483699836</v>
       </c>
       <c r="B5" s="1">
         <f ca="1"/>
-        <v>1.1880147208838956</v>
+        <v>4.9639522752834573</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,16', '1,19')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3,63', '4,96')</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f ca="1"/>
-        <v>9.6202470963632472</v>
+        <v>7.3630006882448278</v>
       </c>
       <c r="B6" s="1">
         <f ca="1"/>
-        <v>5.0116732727571183</v>
+        <v>5.5913692622427984</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('9,62', '5,01')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,36', '5,59')</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f ca="1"/>
-        <v>8.6832662871155932</v>
+        <v>0.59821311964191004</v>
       </c>
       <c r="B7" s="1">
         <f ca="1"/>
-        <v>0.31433286480186595</v>
+        <v>5.7894950028982155</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8,68', '0,31')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,6', '5,79')</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f ca="1"/>
-        <v>5.8404636084957193</v>
+        <v>5.1275963828742146</v>
       </c>
       <c r="B8" s="1">
         <f ca="1"/>
-        <v>0.31317850856775564</v>
+        <v>3.4085261059935323</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,84', '0,31')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,13', '3,41')</v>
       </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f ca="1"/>
-        <v>4.4588806134588417</v>
+        <v>7.2542419185866631</v>
       </c>
       <c r="B9" s="1">
         <f ca="1"/>
-        <v>9.8825428281564829</v>
+        <v>0.77110158103749704</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('4,46', '9,88')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,25', '0,77')</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f ca="1"/>
-        <v>1.1537924204977958</v>
+        <v>6.6058036291149538</v>
       </c>
       <c r="B10" s="1">
         <f ca="1"/>
-        <v>7.1514396976385406</v>
+        <v>9.5432520405198673</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,15', '7,15')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('6,61', '9,54')</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f ca="1"/>
-        <v>2.4792493337756962</v>
+        <v>0.41317033451185381</v>
       </c>
       <c r="B11" s="1">
         <f ca="1"/>
-        <v>5.1721965017034428</v>
+        <v>2.8761335322783239</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2,48', '5,17')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,41', '2,88')</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f ca="1"/>
-        <v>1.3785517613308418</v>
+        <v>4.9268791192098629</v>
       </c>
       <c r="B12" s="1">
         <f ca="1"/>
-        <v>4.3615340791068853</v>
+        <v>2.843883825720086</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,38', '4,36')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('4,93', '2,84')</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f ca="1"/>
-        <v>5.4975956841310385</v>
+        <v>2.808229843787263</v>
       </c>
       <c r="B13" s="1">
         <f ca="1"/>
-        <v>2.3492105855771666</v>
+        <v>2.1913505739775747</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,5', '2,35')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('2,81', '2,19')</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f ca="1"/>
-        <v>7.2196062460593406</v>
+        <v>8.7855724084074929</v>
       </c>
       <c r="B14" s="1">
         <f ca="1"/>
-        <v>2.2830419597811193</v>
+        <v>8.7416857617281885</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,22', '2,28')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8,79', '8,74')</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f ca="1"/>
-        <v>0.83257738895471967</v>
+        <v>7.6142054497506795</v>
       </c>
       <c r="B15" s="1">
         <f ca="1"/>
-        <v>0.68417476986563663</v>
+        <v>5.2636023408392649</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,83', '0,68')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('7,61', '5,26')</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f ca="1"/>
-        <v>0.40974657207961407</v>
+        <v>9.4292002538763811</v>
       </c>
       <c r="B16" s="1">
         <f ca="1"/>
-        <v>5.8050724421605722</v>
+        <v>7.722294430443835</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,41', '5,81')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('9,43', '7,72')</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f ca="1"/>
-        <v>1.1443823984450283</v>
+        <v>8.3952054897730299</v>
       </c>
       <c r="B17" s="1">
         <f ca="1"/>
-        <v>2.8006551805361877</v>
+        <v>7.1866574810746666</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,14', '2,8')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('8,4', '7,19')</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f ca="1"/>
-        <v>5.8815826736123551</v>
+        <v>1.5148743981892405</v>
       </c>
       <c r="B18" s="1">
         <f ca="1"/>
-        <v>6.7608514001746371</v>
+        <v>5.5534445023927148</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,88', '6,76')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,51', '5,55')</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f ca="1"/>
-        <v>5.5798722328422183</v>
+        <v>3.3541120828933497</v>
       </c>
       <c r="B19" s="1">
         <f ca="1"/>
-        <v>0.58338364690580136</v>
+        <v>0.64811813086214443</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('5,58', '0,58')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3,35', '0,65')</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f ca="1"/>
-        <v>6.9060563008237708</v>
+        <v>0.62016438453210476</v>
       </c>
       <c r="B20" s="1">
         <f ca="1"/>
-        <v>1.8253006400313758</v>
+        <v>1.4564992748810255</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('6,91', '1,83')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('0,62', '1,46')</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f ca="1"/>
-        <v>1.4072535534143213</v>
+        <v>3.2845809932757657</v>
       </c>
       <c r="B21" s="1">
         <f ca="1"/>
-        <v>2.2513880605009096</v>
+        <v>9.5904137787966679</v>
       </c>
       <c r="D21" t="str">
         <f ca="1">_xlfn.CONCAT("INSERT INTO Punto (xCoord,yCoord) VALUES ('",ROUND(A21,2),"', '",ROUND(B21,2),"')")</f>
-        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('1,41', '2,25')</v>
+        <v>INSERT INTO Punto (xCoord,yCoord) VALUES ('3,28', '9,59')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>